<commit_message>
Why is my data gone?
Some data disappeared, so I added them back!
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuanx\Documents\GitHub\ThreeBody\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7E1AD9FE-E276-483C-B263-7D115529B436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D626045-57F9-464D-B499-4CEC156B14BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>x1</t>
   </si>
@@ -104,13 +115,25 @@
   </si>
   <si>
     <t>II.C.3b yin-yang II</t>
+  </si>
+  <si>
+    <t>m1</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>Mass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,12 +275,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -266,7 +283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,18 +461,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -620,12 +625,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -633,38 +634,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -711,41 +714,11 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -762,6 +735,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -809,7 +806,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -821,6 +818,48 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1140,875 +1179,1023 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="9" width="8.7265625" style="13"/>
-    <col min="10" max="10" width="8.7265625" style="13" customWidth="1"/>
-    <col min="11" max="13" width="8.7265625" style="13"/>
-    <col min="14" max="14" width="34.6328125" style="13" customWidth="1"/>
-    <col min="15" max="15" width="15.08984375" style="13" customWidth="1"/>
-    <col min="16" max="16384" width="8.7265625" style="13"/>
+    <col min="1" max="2" width="8.7265625" style="3"/>
+    <col min="3" max="3" width="8.7265625" style="3" customWidth="1"/>
+    <col min="4" max="9" width="8.7265625" style="3"/>
+    <col min="10" max="10" width="8.7265625" style="3" customWidth="1"/>
+    <col min="11" max="16" width="8.7265625" style="3"/>
+    <col min="17" max="17" width="34.6328125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="15.08984375" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:18" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="5" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="13"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="6"/>
-    </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+    </row>
+    <row r="2" spans="1:18" s="2" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="Q2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="R2" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
-        <v>0</v>
-      </c>
-      <c r="G3" s="13">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
         <v>0.30689</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="3">
         <v>0.12551000000000001</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="2">
         <f>G3</f>
         <v>0.30689</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="2">
         <f>H3</f>
         <v>0.12551000000000001</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="2">
         <f>-2*G3</f>
         <v>-0.61377999999999999</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="2">
         <f>-2*H3</f>
         <v>-0.25102000000000002</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1</v>
+      </c>
+      <c r="P3" s="2">
         <v>6.2355999999999998</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="Q3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="R3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B4" s="12">
-        <v>0</v>
-      </c>
-      <c r="C4" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12">
-        <v>0</v>
-      </c>
-      <c r="F4" s="12">
-        <v>0</v>
-      </c>
-      <c r="G4" s="13">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
         <v>0.39295000000000002</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="3">
         <v>9.758E-2</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="2">
         <f t="shared" ref="I4:I17" si="0">G4</f>
         <v>0.39295000000000002</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="2">
         <f t="shared" ref="J4:J17" si="1">H4</f>
         <v>9.758E-2</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="2">
         <f t="shared" ref="K4:K17" si="2">-2*G4</f>
         <v>-0.78590000000000004</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="2">
         <f t="shared" ref="L4:L17" si="3">-2*H4</f>
         <v>-0.19516</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1</v>
+      </c>
+      <c r="P4" s="2">
         <v>7.0038999999999998</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="16" t="s">
+      <c r="Q4" s="8"/>
+      <c r="R4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B5" s="12">
-        <v>0</v>
-      </c>
-      <c r="C5" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="12">
-        <v>0</v>
-      </c>
-      <c r="E5" s="12">
-        <v>0</v>
-      </c>
-      <c r="F5" s="12">
-        <v>0</v>
-      </c>
-      <c r="G5" s="13">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
         <v>0.18428</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="3">
         <v>0.58718999999999999</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="2">
         <f t="shared" si="0"/>
         <v>0.18428</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="2">
         <f t="shared" si="1"/>
         <v>0.58718999999999999</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="2">
         <f t="shared" si="2"/>
         <v>-0.36856</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="2">
         <f t="shared" si="3"/>
         <v>-1.17438</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
+      <c r="P5" s="2">
         <v>63.534500000000001</v>
       </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="16" t="s">
+      <c r="Q5" s="8"/>
+      <c r="R5" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B6" s="12">
-        <v>0</v>
-      </c>
-      <c r="C6" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0</v>
-      </c>
-      <c r="E6" s="12">
-        <v>0</v>
-      </c>
-      <c r="F6" s="12">
-        <v>0</v>
-      </c>
-      <c r="G6" s="13">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
         <v>0.46444000000000002</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="3">
         <v>0.39606000000000002</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="2">
         <f t="shared" si="0"/>
         <v>0.46444000000000002</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="2">
         <f t="shared" si="1"/>
         <v>0.39606000000000002</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="2">
         <f t="shared" si="2"/>
         <v>-0.92888000000000004</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="2">
         <f t="shared" si="3"/>
         <v>-0.79212000000000005</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2">
+        <v>1</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1</v>
+      </c>
+      <c r="P6" s="4">
         <v>14.8939</v>
       </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="16" t="s">
+      <c r="Q6" s="8"/>
+      <c r="R6" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B7" s="12">
-        <v>0</v>
-      </c>
-      <c r="C7" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D7" s="12">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12">
-        <v>0</v>
-      </c>
-      <c r="F7" s="12">
-        <v>0</v>
-      </c>
-      <c r="G7" s="13">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
         <v>0.43917</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="3">
         <v>0.45296999999999998</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="2">
         <f t="shared" si="0"/>
         <v>0.43917</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="2">
         <f t="shared" si="1"/>
         <v>0.45296999999999998</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="2">
         <f t="shared" si="2"/>
         <v>-0.87834000000000001</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="2">
         <f t="shared" si="3"/>
         <v>-0.90593999999999997</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="2">
+        <v>1</v>
+      </c>
+      <c r="N7" s="2">
+        <v>1</v>
+      </c>
+      <c r="O7" s="2">
+        <v>1</v>
+      </c>
+      <c r="P7" s="4">
         <v>28.670300000000001</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="16" t="s">
+      <c r="Q7" s="8"/>
+      <c r="R7" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B8" s="12">
-        <v>0</v>
-      </c>
-      <c r="C8" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D8" s="12">
-        <v>0</v>
-      </c>
-      <c r="E8" s="12">
-        <v>0</v>
-      </c>
-      <c r="F8" s="12">
-        <v>0</v>
-      </c>
-      <c r="G8" s="13">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
         <v>0.40592</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="3">
         <v>0.23016</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="2">
         <f t="shared" si="0"/>
         <v>0.40592</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="2">
         <f t="shared" si="1"/>
         <v>0.23016</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="2">
         <f t="shared" si="2"/>
         <v>-0.81184000000000001</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="2">
         <f t="shared" si="3"/>
         <v>-0.46032000000000001</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2">
+        <v>1</v>
+      </c>
+      <c r="O8" s="2">
+        <v>1</v>
+      </c>
+      <c r="P8" s="3">
         <v>13.8658</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="16" t="s">
+      <c r="Q8" s="8"/>
+      <c r="R8" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B9" s="12">
-        <v>0</v>
-      </c>
-      <c r="C9" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D9" s="12">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12">
-        <v>0</v>
-      </c>
-      <c r="F9" s="12">
-        <v>0</v>
-      </c>
-      <c r="G9" s="13">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
         <v>0.38344</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="3">
         <v>0.37735999999999997</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="2">
         <f t="shared" si="0"/>
         <v>0.38344</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="2">
         <f t="shared" si="1"/>
         <v>0.37735999999999997</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="2">
         <f t="shared" si="2"/>
         <v>-0.76688000000000001</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="2">
         <f t="shared" si="3"/>
         <v>-0.75471999999999995</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="2">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2">
+        <v>1</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1</v>
+      </c>
+      <c r="P9" s="3">
         <v>25.840599999999998</v>
       </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="16" t="s">
+      <c r="Q9" s="8"/>
+      <c r="R9" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B10" s="12">
-        <v>0</v>
-      </c>
-      <c r="C10" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D10" s="12">
-        <v>0</v>
-      </c>
-      <c r="E10" s="12">
-        <v>0</v>
-      </c>
-      <c r="F10" s="12">
-        <v>0</v>
-      </c>
-      <c r="G10" s="13">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="3">
         <v>0.12789</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="2">
         <f t="shared" si="0"/>
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="2">
         <f t="shared" si="1"/>
         <v>0.12789</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="2">
         <f t="shared" si="2"/>
         <v>-0.1666</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="2">
         <f t="shared" si="3"/>
         <v>-0.25578000000000001</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="2">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2">
+        <v>1</v>
+      </c>
+      <c r="O10" s="2">
+        <v>1</v>
+      </c>
+      <c r="P10" s="3">
         <v>10.466799999999999</v>
       </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="16" t="s">
+      <c r="Q10" s="8"/>
+      <c r="R10" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B11" s="12">
-        <v>0</v>
-      </c>
-      <c r="C11" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D11" s="12">
-        <v>0</v>
-      </c>
-      <c r="E11" s="12">
-        <v>0</v>
-      </c>
-      <c r="F11" s="12">
-        <v>0</v>
-      </c>
-      <c r="G11" s="13">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
         <v>0.35011199999999998</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="3">
         <v>7.9339999999999994E-2</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="2">
         <f t="shared" si="0"/>
         <v>0.35011199999999998</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="2">
         <f t="shared" si="1"/>
         <v>7.9339999999999994E-2</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="2">
         <f t="shared" si="2"/>
         <v>-0.70022399999999996</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="2">
         <f t="shared" si="3"/>
         <v>-0.15867999999999999</v>
       </c>
-      <c r="M11" s="13">
+      <c r="M11" s="2">
+        <v>1</v>
+      </c>
+      <c r="N11" s="2">
+        <v>1</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1</v>
+      </c>
+      <c r="P11" s="3">
         <v>79.475899999999996</v>
       </c>
-      <c r="N11" s="2"/>
-      <c r="O11" s="16" t="s">
+      <c r="Q11" s="8"/>
+      <c r="R11" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B12" s="12">
-        <v>0</v>
-      </c>
-      <c r="C12" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D12" s="12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="12">
-        <v>0</v>
-      </c>
-      <c r="F12" s="12">
-        <v>0</v>
-      </c>
-      <c r="G12" s="13">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
         <v>8.0579999999999999E-2</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="3">
         <v>0.58884000000000003</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="2">
         <f t="shared" si="0"/>
         <v>8.0579999999999999E-2</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="2">
         <f t="shared" si="1"/>
         <v>0.58884000000000003</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="2">
         <f t="shared" si="2"/>
         <v>-0.16116</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="2">
         <f t="shared" si="3"/>
         <v>-1.1776800000000001</v>
       </c>
-      <c r="M12" s="13">
+      <c r="M12" s="2">
+        <v>1</v>
+      </c>
+      <c r="N12" s="2">
+        <v>1</v>
+      </c>
+      <c r="O12" s="2">
+        <v>1</v>
+      </c>
+      <c r="P12" s="3">
         <v>21.271000000000001</v>
       </c>
-      <c r="N12" s="2"/>
-      <c r="O12" s="16" t="s">
+      <c r="Q12" s="8"/>
+      <c r="R12" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B13" s="12">
-        <v>0</v>
-      </c>
-      <c r="C13" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D13" s="12">
-        <v>0</v>
-      </c>
-      <c r="E13" s="12">
-        <v>0</v>
-      </c>
-      <c r="F13" s="12">
-        <v>0</v>
-      </c>
-      <c r="G13" s="13">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
         <v>0.55906</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="3">
         <v>0.34919</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="2">
         <f t="shared" si="0"/>
         <v>0.55906</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="2">
         <f t="shared" si="1"/>
         <v>0.34919</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="2">
         <f t="shared" si="2"/>
         <v>-1.11812</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="2">
         <f t="shared" si="3"/>
         <v>-0.69838</v>
       </c>
-      <c r="M13" s="13">
+      <c r="M13" s="2">
+        <v>1</v>
+      </c>
+      <c r="N13" s="2">
+        <v>1</v>
+      </c>
+      <c r="O13" s="2">
+        <v>1</v>
+      </c>
+      <c r="P13" s="3">
         <v>55.501800000000003</v>
       </c>
-      <c r="N13" s="2"/>
-      <c r="O13" s="16" t="s">
+      <c r="Q13" s="8"/>
+      <c r="R13" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B14" s="12">
-        <v>0</v>
-      </c>
-      <c r="C14" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D14" s="12">
-        <v>0</v>
-      </c>
-      <c r="E14" s="12">
-        <v>0</v>
-      </c>
-      <c r="F14" s="12">
-        <v>0</v>
-      </c>
-      <c r="G14" s="13">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
         <v>0.51393999999999995</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="3">
         <v>0.30474000000000001</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="2">
         <f t="shared" si="0"/>
         <v>0.51393999999999995</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="2">
         <f t="shared" si="1"/>
         <v>0.30474000000000001</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="2">
         <f t="shared" si="2"/>
         <v>-1.0278799999999999</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="2">
         <f t="shared" si="3"/>
         <v>-0.60948000000000002</v>
       </c>
-      <c r="M14" s="13">
+      <c r="M14" s="2">
+        <v>1</v>
+      </c>
+      <c r="N14" s="2">
+        <v>1</v>
+      </c>
+      <c r="O14" s="2">
+        <v>1</v>
+      </c>
+      <c r="P14" s="3">
         <v>17.328399999999998</v>
       </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="16" t="s">
+      <c r="Q14" s="8"/>
+      <c r="R14" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B15" s="12">
-        <v>0</v>
-      </c>
-      <c r="C15" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D15" s="12">
-        <v>0</v>
-      </c>
-      <c r="E15" s="12">
-        <v>0</v>
-      </c>
-      <c r="F15" s="12">
-        <v>0</v>
-      </c>
-      <c r="G15" s="13">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
         <v>0.28270000000000001</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="3">
         <v>0.32721</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="2">
         <f t="shared" si="0"/>
         <v>0.28270000000000001</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="2">
         <f t="shared" si="1"/>
         <v>0.32721</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="2">
         <f t="shared" si="2"/>
         <v>-0.56540000000000001</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="2">
         <f t="shared" si="3"/>
         <v>-0.65442</v>
       </c>
-      <c r="M15" s="13">
+      <c r="M15" s="2">
+        <v>1</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1</v>
+      </c>
+      <c r="O15" s="2">
+        <v>1</v>
+      </c>
+      <c r="P15" s="3">
         <v>10.9626</v>
       </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="16" t="s">
+      <c r="Q15" s="8"/>
+      <c r="R15" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A16" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B16" s="12">
-        <v>0</v>
-      </c>
-      <c r="C16" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D16" s="12">
-        <v>0</v>
-      </c>
-      <c r="E16" s="12">
-        <v>0</v>
-      </c>
-      <c r="F16" s="12">
-        <v>0</v>
-      </c>
-      <c r="G16" s="13">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
         <v>0.41682000000000002</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="3">
         <v>0.33033000000000001</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="2">
         <f t="shared" si="0"/>
         <v>0.41682000000000002</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="2">
         <f t="shared" si="1"/>
         <v>0.33033000000000001</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="2">
         <f t="shared" si="2"/>
         <v>-0.83364000000000005</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="2">
         <f t="shared" si="3"/>
         <v>-0.66066000000000003</v>
       </c>
-      <c r="M16" s="13">
+      <c r="M16" s="2">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2">
+        <v>1</v>
+      </c>
+      <c r="O16" s="2">
+        <v>1</v>
+      </c>
+      <c r="P16" s="3">
         <v>55.7898</v>
       </c>
-      <c r="N16" s="2"/>
-      <c r="O16" s="16" t="s">
+      <c r="Q16" s="8"/>
+      <c r="R16" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A17" s="12">
-        <v>-1</v>
-      </c>
-      <c r="B17" s="12">
-        <v>0</v>
-      </c>
-      <c r="C17" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D17" s="12">
-        <v>0</v>
-      </c>
-      <c r="E17" s="12">
-        <v>0</v>
-      </c>
-      <c r="F17" s="12">
-        <v>0</v>
-      </c>
-      <c r="G17" s="13">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
         <v>0.41733999999999999</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="3">
         <v>0.31309999999999999</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="2">
         <f t="shared" si="0"/>
         <v>0.41733999999999999</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="2">
         <f t="shared" si="1"/>
         <v>0.31309999999999999</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="2">
         <f t="shared" si="2"/>
         <v>-0.83467999999999998</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L17" s="2">
         <f t="shared" si="3"/>
         <v>-0.62619999999999998</v>
       </c>
-      <c r="M17" s="13">
+      <c r="M17" s="2">
+        <v>1</v>
+      </c>
+      <c r="N17" s="2">
+        <v>1</v>
+      </c>
+      <c r="O17" s="2">
+        <v>1</v>
+      </c>
+      <c r="P17" s="3">
         <v>54.207599999999999</v>
       </c>
-      <c r="N17" s="2"/>
-      <c r="O17" s="16" t="s">
+      <c r="Q17" s="8"/>
+      <c r="R17" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="O21" s="16"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="O22" s="16"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="O23" s="16"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="O24" s="16"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="O25" s="16"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="O26" s="16"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="O27" s="16"/>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R21" s="6"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R22" s="6"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R23" s="6"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R24" s="6"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R25" s="6"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R26" s="6"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R27" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:L1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="Q3:Q17"/>
     <mergeCell ref="M1:O1"/>
-    <mergeCell ref="N3:N17"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="M2:M1048576 K2:K1048576 I2:I1048576 G2:G1048576 E2:E1048576 C2:C1048576 A2:A1048576 O2:O17 O19:O1048576">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+  <conditionalFormatting sqref="A2:A1048576 C2:C1048576 E2:E1048576 G2:G1048576 I2:I1048576 K2:K1048576 M2:M1048576 O2:O1048576 Q2:Q1048576">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
-    <cfRule type="expression" priority="3">
-      <formula>"AND(ROW(A2)%2=1, NOT(ISBLANK(A2))"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O17 O19:O1048576">
+  <conditionalFormatting sqref="Q1:R1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1"/>
+    <hyperlink ref="Q3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>